<commit_message>
Reorg. and changed the license and modified readme.
</commit_message>
<xml_diff>
--- a/Spot_Outcomes.xlsx
+++ b/Spot_Outcomes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jens/Documents/Python/hydrOpt/dynProg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jens/Documents/Python/dynprog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB8F0F4-6492-444E-A4D2-9B89AC3B4BF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F38324-CC01-D941-A784-F43BACED17C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="460" windowWidth="21320" windowHeight="17100" xr2:uid="{97F7539C-452B-A548-92BB-3CE594F78CD0}"/>
   </bookViews>
@@ -2453,8 +2453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2513C063-BB01-5E4E-BC20-809D3836ED8C}">
   <dimension ref="A1:D271"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C264" sqref="C264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3724,7 +3724,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>43938.708328182867</v>
+        <v>43938.708328645836</v>
       </c>
       <c r="B91">
         <v>23.82</v>
@@ -3738,7 +3738,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>43938.749994791666</v>
+        <v>43938.749995312501</v>
       </c>
       <c r="B92">
         <v>26.42</v>
@@ -3752,7 +3752,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <v>43938.791661400464</v>
+        <v>43938.791661979165</v>
       </c>
       <c r="B93">
         <v>26.45</v>
@@ -3766,7 +3766,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>43938.833328009256</v>
+        <v>43938.833328645836</v>
       </c>
       <c r="B94">
         <v>27</v>
@@ -3780,7 +3780,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <v>43938.874994618054</v>
+        <v>43938.874995312501</v>
       </c>
       <c r="B95">
         <v>27.26</v>
@@ -3794,7 +3794,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <v>43938.916661226853</v>
+        <v>43938.916661979165</v>
       </c>
       <c r="B96">
         <v>23.7</v>
@@ -3808,7 +3808,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
-        <v>43938.958327835651</v>
+        <v>43938.958328645836</v>
       </c>
       <c r="B97">
         <v>20.12</v>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
-        <v>43938.999994444443</v>
+        <v>43938.999995312501</v>
       </c>
       <c r="B98">
         <v>22.05</v>
@@ -3836,7 +3836,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
-        <v>43939.041661053241</v>
+        <v>43939.041661979165</v>
       </c>
       <c r="B99">
         <v>21.9</v>
@@ -3850,7 +3850,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <v>43939.08332766204</v>
+        <v>43939.083328645836</v>
       </c>
       <c r="B100">
         <v>21.47</v>
@@ -3864,7 +3864,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <v>43939.124994270831</v>
+        <v>43939.124995312501</v>
       </c>
       <c r="B101">
         <v>21.06</v>
@@ -3878,7 +3878,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>43939.166660879629</v>
+        <v>43939.166661979165</v>
       </c>
       <c r="B102">
         <v>20.22</v>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>43939.208327488428</v>
+        <v>43939.208328645836</v>
       </c>
       <c r="B103">
         <v>20.71</v>
@@ -3906,7 +3906,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>43939.249994097219</v>
+        <v>43939.249995312501</v>
       </c>
       <c r="B104">
         <v>21.16</v>
@@ -3920,7 +3920,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>43939.291660706018</v>
+        <v>43939.291661979165</v>
       </c>
       <c r="B105">
         <v>22.02</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <v>43939.333327314816</v>
+        <v>43939.333328645836</v>
       </c>
       <c r="B106">
         <v>22.55</v>
@@ -3948,7 +3948,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <v>43939.374993923608</v>
+        <v>43939.374995312501</v>
       </c>
       <c r="B107">
         <v>21.75</v>
@@ -3962,7 +3962,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>43939.416660532406</v>
+        <v>43939.416661979165</v>
       </c>
       <c r="B108">
         <v>18.04</v>
@@ -3976,7 +3976,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <v>43939.458327141205</v>
+        <v>43939.458328645836</v>
       </c>
       <c r="B109">
         <v>15.94</v>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>43939.499993750003</v>
+        <v>43939.499995312501</v>
       </c>
       <c r="B110">
         <v>14.84</v>
@@ -4004,7 +4004,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
-        <v>43939.541660358795</v>
+        <v>43939.541661979165</v>
       </c>
       <c r="B111">
         <v>12.5</v>
@@ -4018,7 +4018,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
-        <v>43939.583326967593</v>
+        <v>43939.583328645836</v>
       </c>
       <c r="B112">
         <v>10.43</v>
@@ -4032,7 +4032,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
-        <v>43939.624993576392</v>
+        <v>43939.624995312501</v>
       </c>
       <c r="B113">
         <v>11.45</v>
@@ -4046,7 +4046,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
-        <v>43939.666660185183</v>
+        <v>43939.666661979165</v>
       </c>
       <c r="B114">
         <v>14.88</v>
@@ -4060,7 +4060,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
-        <v>43939.708326793982</v>
+        <v>43939.708328645836</v>
       </c>
       <c r="B115">
         <v>18.77</v>
@@ -4074,7 +4074,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
-        <v>43939.74999340278</v>
+        <v>43939.749995312501</v>
       </c>
       <c r="B116">
         <v>23.92</v>
@@ -4088,7 +4088,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
-        <v>43939.791660011571</v>
+        <v>43939.791661979165</v>
       </c>
       <c r="B117">
         <v>23.98</v>
@@ -4102,7 +4102,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
-        <v>43939.83332662037</v>
+        <v>43939.833328645836</v>
       </c>
       <c r="B118">
         <v>24.46</v>
@@ -4116,7 +4116,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
-        <v>43939.874993229168</v>
+        <v>43939.874995312501</v>
       </c>
       <c r="B119">
         <v>22.82</v>
@@ -4130,7 +4130,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
-        <v>43939.91665983796</v>
+        <v>43939.916661979165</v>
       </c>
       <c r="B120">
         <v>22.31</v>
@@ -4144,7 +4144,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
-        <v>43939.958326446758</v>
+        <v>43939.958328645836</v>
       </c>
       <c r="B121">
         <v>19.309999999999999</v>
@@ -4158,752 +4158,752 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
-        <v>43939.999993055557</v>
+        <v>43939.999995312501</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
-        <v>43940.041659664355</v>
+        <v>43940.041661979165</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
-        <v>43940.083326273147</v>
+        <v>43940.083328645836</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
-        <v>43940.124992881945</v>
+        <v>43940.124995312501</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
-        <v>43940.166659490744</v>
+        <v>43940.166661979165</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
-        <v>43940.208326099535</v>
+        <v>43940.208328645836</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
-        <v>43940.249992708334</v>
+        <v>43940.249995312501</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
-        <v>43940.291659317132</v>
+        <v>43940.291661979165</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
-        <v>43940.333325925923</v>
+        <v>43940.333328645836</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
-        <v>43940.374992534722</v>
+        <v>43940.374995312501</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
-        <v>43940.416659143521</v>
+        <v>43940.416661979165</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
-        <v>43940.458325752312</v>
+        <v>43940.458328645836</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
-        <v>43940.49999236111</v>
+        <v>43940.499995312501</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
-        <v>43940.541658969909</v>
+        <v>43940.541661979165</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
-        <v>43940.5833255787</v>
+        <v>43940.583328645836</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
-        <v>43940.624992187499</v>
+        <v>43940.624995312501</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
-        <v>43940.666658796297</v>
+        <v>43940.666661979165</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
-        <v>43940.708325405096</v>
+        <v>43940.708328645836</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
-        <v>43940.749992013887</v>
+        <v>43940.749995312501</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
-        <v>43940.791658622686</v>
+        <v>43940.791661979165</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
-        <v>43940.833325231484</v>
+        <v>43940.833328645836</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
-        <v>43940.874991840275</v>
+        <v>43940.874995312501</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
-        <v>43940.916658449074</v>
+        <v>43940.916661979165</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>43940.958325057873</v>
+        <v>43940.958328645836</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
-        <v>43940.999991666664</v>
+        <v>43940.999995312501</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>43941.041658275462</v>
+        <v>43941.041661979165</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
-        <v>43941.083324884261</v>
+        <v>43941.083328645836</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
-        <v>43941.124991493052</v>
+        <v>43941.124995312501</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
-        <v>43941.166658101851</v>
+        <v>43941.166661979165</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
-        <v>43941.208324710649</v>
+        <v>43941.208328645836</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
-        <v>43941.249991319448</v>
+        <v>43941.249995312501</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
-        <v>43941.291657928239</v>
+        <v>43941.291661979165</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
-        <v>43941.333324537038</v>
+        <v>43941.333328645836</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
-        <v>43941.374991145836</v>
+        <v>43941.374995312501</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
-        <v>43941.416657754628</v>
+        <v>43941.416661979165</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
-        <v>43941.458324363426</v>
+        <v>43941.458328645836</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
-        <v>43941.499990972225</v>
+        <v>43941.499995312501</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
-        <v>43941.541657581016</v>
+        <v>43941.541661979165</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
-        <v>43941.583324189814</v>
+        <v>43941.583328645836</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
-        <v>43941.624990798613</v>
+        <v>43941.624995312501</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
-        <v>43941.666657407404</v>
+        <v>43941.666661979165</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
-        <v>43941.708324016203</v>
+        <v>43941.708328645836</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
-        <v>43941.749990625001</v>
+        <v>43941.749995312501</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>43941.7916572338</v>
+        <v>43941.791661979165</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
-        <v>43941.833323842591</v>
+        <v>43941.833328645836</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
-        <v>43941.87499045139</v>
+        <v>43941.874995312501</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
-        <v>43941.916657060188</v>
+        <v>43941.916661979165</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
-        <v>43941.95832366898</v>
+        <v>43941.958328645836</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
-        <v>43941.999990277778</v>
+        <v>43941.999995312501</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
-        <v>43942.041656886577</v>
+        <v>43942.041661979165</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
-        <v>43942.083323495368</v>
+        <v>43942.083328645836</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
-        <v>43942.124990104166</v>
+        <v>43942.124995312501</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
-        <v>43942.166656712965</v>
+        <v>43942.166661979165</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
-        <v>43942.208323321756</v>
+        <v>43942.208328645836</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
-        <v>43942.249989930555</v>
+        <v>43942.249995312501</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
-        <v>43942.291656539353</v>
+        <v>43942.291661979165</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
-        <v>43942.333323148145</v>
+        <v>43942.333328645836</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
-        <v>43942.374989756943</v>
+        <v>43942.374995312501</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
-        <v>43942.416656365742</v>
+        <v>43942.416661979165</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
-        <v>43942.45832297454</v>
+        <v>43942.458328645836</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
-        <v>43942.499989583332</v>
+        <v>43942.499995312501</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
-        <v>43942.54165619213</v>
+        <v>43942.541661979165</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
-        <v>43942.583322800929</v>
+        <v>43942.583328645836</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
-        <v>43942.62498940972</v>
+        <v>43942.624995312501</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
-        <v>43942.666656018519</v>
+        <v>43942.666661979165</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
-        <v>43942.708322627317</v>
+        <v>43942.708328645836</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
-        <v>43942.749989236108</v>
+        <v>43942.749995312501</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
-        <v>43942.791655844907</v>
+        <v>43942.791661979165</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
-        <v>43942.833322453705</v>
+        <v>43942.833328645836</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
-        <v>43942.874989062497</v>
+        <v>43942.874995312501</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
-        <v>43942.916655671295</v>
+        <v>43942.916661979165</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
-        <v>43942.958322280094</v>
+        <v>43942.958328645836</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
-        <v>43942.999988888892</v>
+        <v>43942.999995312501</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
-        <v>43943.041655497684</v>
+        <v>43943.041661979165</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
-        <v>43943.083322106482</v>
+        <v>43943.083328645836</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
-        <v>43943.124988715281</v>
+        <v>43943.124995312501</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
-        <v>43943.166655324072</v>
+        <v>43943.166661979165</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
-        <v>43943.208321932871</v>
+        <v>43943.208328645836</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
-        <v>43943.249988541669</v>
+        <v>43943.249995312501</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
-        <v>43943.29165515046</v>
+        <v>43943.291661979165</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
-        <v>43943.333321759259</v>
+        <v>43943.333328645836</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
-        <v>43943.374988368058</v>
+        <v>43943.374995312501</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
-        <v>43943.416654976849</v>
+        <v>43943.416661979165</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
-        <v>43943.458321585647</v>
+        <v>43943.458328645836</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
-        <v>43943.499988194446</v>
+        <v>43943.499995312501</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
-        <v>43943.541654803237</v>
+        <v>43943.541661979165</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
-        <v>43943.583321412036</v>
+        <v>43943.583328645836</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
-        <v>43943.624988020834</v>
+        <v>43943.624995312501</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
-        <v>43943.666654629633</v>
+        <v>43943.666661979165</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
-        <v>43943.708321238424</v>
+        <v>43943.708328645836</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
-        <v>43943.749987847223</v>
+        <v>43943.749995312501</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
-        <v>43943.791654456021</v>
+        <v>43943.791661979165</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
-        <v>43943.833321064812</v>
+        <v>43943.833328645836</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
-        <v>43943.874987673611</v>
+        <v>43943.874995312501</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
-        <v>43943.91665428241</v>
+        <v>43943.916661979165</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
-        <v>43943.958320891201</v>
+        <v>43943.958328645836</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
-        <v>43943.999987499999</v>
+        <v>43943.999995312501</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
-        <v>43944.041654108798</v>
+        <v>43944.041661979165</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
-        <v>43944.083320717589</v>
+        <v>43944.083328645836</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
-        <v>43944.124987326388</v>
+        <v>43944.124995312501</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
-        <v>43944.166653935186</v>
+        <v>43944.166661979165</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
-        <v>43944.208320543985</v>
+        <v>43944.208328645836</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
-        <v>43944.249987152776</v>
+        <v>43944.249995312501</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
-        <v>43944.291653761575</v>
+        <v>43944.291661979165</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
-        <v>43944.333320370373</v>
+        <v>43944.333328645836</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
-        <v>43944.374986979165</v>
+        <v>43944.374995312501</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
-        <v>43944.416653587963</v>
+        <v>43944.416661979165</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
-        <v>43944.458320196762</v>
+        <v>43944.458328645836</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
-        <v>43944.499986805553</v>
+        <v>43944.499995312501</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
-        <v>43944.541653414351</v>
+        <v>43944.541661979165</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
-        <v>43944.58332002315</v>
+        <v>43944.583328645836</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
-        <v>43944.624986631941</v>
+        <v>43944.624995312501</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
-        <v>43944.66665324074</v>
+        <v>43944.666661979165</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
-        <v>43944.708319849538</v>
+        <v>43944.708328645836</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
-        <v>43944.749986458337</v>
+        <v>43944.749995312501</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
-        <v>43944.791653067128</v>
+        <v>43944.791661979165</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
-        <v>43944.833319675927</v>
+        <v>43944.833328645836</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
-        <v>43944.874986284725</v>
+        <v>43944.874995312501</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
-        <v>43944.916652893517</v>
+        <v>43944.916661979165</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
-        <v>43944.958319502315</v>
+        <v>43944.958328645836</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
-        <v>43944.999986111114</v>
+        <v>43944.999995312501</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
-        <v>43945.041652719905</v>
+        <v>43945.041661979165</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
-        <v>43945.083319328704</v>
+        <v>43945.083328645836</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
-        <v>43945.124985937502</v>
+        <v>43945.124995312501</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
-        <v>43945.166652546293</v>
+        <v>43945.166661979165</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
-        <v>43945.208319155092</v>
+        <v>43945.208328645836</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
-        <v>43945.24998576389</v>
+        <v>43945.249995312501</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
-        <v>43945.291652372682</v>
+        <v>43945.291661979165</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
-        <v>43945.33331898148</v>
+        <v>43945.333328645836</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
-        <v>43945.374985590279</v>
+        <v>43945.374995312501</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
-        <v>43945.416652199077</v>
+        <v>43945.416661979165</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
-        <v>43945.458318807869</v>
+        <v>43945.458328645836</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
-        <v>43945.499985416667</v>
+        <v>43945.499995312501</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
-        <v>43945.541652025466</v>
+        <v>43945.541661979165</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
-        <v>43945.583318634257</v>
+        <v>43945.583328645836</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
-        <v>43945.624985243056</v>
+        <v>43945.624995312501</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
-        <v>43945.666651851854</v>
+        <v>43945.666661979165</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
-        <v>43945.708318460645</v>
+        <v>43945.708328645836</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
-        <v>43945.749985069444</v>
+        <v>43945.749995312501</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
-        <v>43945.791651678242</v>
+        <v>43945.791661979165</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
-        <v>43945.833318287034</v>
+        <v>43945.833328645836</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
-        <v>43945.874984895832</v>
+        <v>43945.874995312501</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
-        <v>43945.916651504631</v>
+        <v>43945.916661979165</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
-        <v>43945.958318113429</v>
+        <v>43945.958328645836</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
-        <v>43945.999984722221</v>
+        <v>43945.999995312501</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
-        <v>43946.041651331019</v>
+        <v>43946.041661979165</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
-        <v>43946.083317939818</v>
+        <v>43946.083328645836</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
-        <v>43946.124984548609</v>
+        <v>43946.124995312501</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
-        <v>43946.166651157408</v>
+        <v>43946.166661979165</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
-        <v>43946.208317766206</v>
+        <v>43946.208328645836</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed attr. names in Basin class
</commit_message>
<xml_diff>
--- a/Spot_Outcomes.xlsx
+++ b/Spot_Outcomes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jens/Documents/Python/dynprog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F38324-CC01-D941-A784-F43BACED17C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1248E23-E9DA-8549-9864-91F7E513D9D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="460" windowWidth="21320" windowHeight="17100" xr2:uid="{97F7539C-452B-A548-92BB-3CE594F78CD0}"/>
   </bookViews>
@@ -542,6 +542,150 @@
                 <c:pt idx="119">
                   <c:v>19.309999999999999</c:v>
                 </c:pt>
+                <c:pt idx="144">
+                  <c:v>8.4700000000000006</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>6.49</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>4.67</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>3.98</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>4.17</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>9.02</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>18.940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>22.37</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>21.94</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>14.94</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>13.52</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>9.08</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>6.24</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>12.84</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>15.13</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>20.41</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>21.6</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>18.670000000000002</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>13.19</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>4.72</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>4.29</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>1.28</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>-1.89</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>-0.61</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>8.2799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>13.68</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>17.28</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>17.03</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>14.68</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>13.24</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>14.69</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>12.94</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>13.92</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>8.6199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>13.86</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>16.46</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>13.01</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>13.69</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>9.07</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -944,6 +1088,150 @@
                 <c:pt idx="119">
                   <c:v>18.38</c:v>
                 </c:pt>
+                <c:pt idx="144">
+                  <c:v>4.43</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>4.38</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>3.69</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>4.78</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>22.82</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>22.93</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>16.07</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>11.72</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>-4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>-29.7</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>-44.25</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>-39.49</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>-23.71</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>16.38</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>17.809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>18.38</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>14.05</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>10.28</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>4.8499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>4.6500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>4.3099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>3.69</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>-0.59</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>3.72</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>4.7300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>16.13</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>16.52</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>7.92</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>-19.21</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>-69.05</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>-79.739999999999995</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>-80.09</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>-83.94</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>-80.02</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>-78.09</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>-23.12</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>5.53</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>11.17</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>8.31</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1345,6 +1633,150 @@
                 </c:pt>
                 <c:pt idx="119">
                   <c:v>18.8</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>4.43</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>4.38</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>3.69</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>4.7699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>9.16</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>12.77</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>13.97</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>12.02</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>6.91</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>1.54</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>-0.09</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>-22.96</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>-23.12</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>-14.63</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>14.23</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>15.02</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>15.81</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>14.05</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>13.39</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>6.31</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>4.3499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>3.73</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>3.72</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>4.7300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>11.43</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>11.17</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>8.33</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>-8.65</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>-3.33</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>-0.92</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>-3.99</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>-8.44</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>-0.09</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>11.17</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>9.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2453,8 +2885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2513C063-BB01-5E4E-BC20-809D3836ED8C}">
   <dimension ref="A1:D271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C264" sqref="C264"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4271,322 +4703,754 @@
         <v>43940.916661979165</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>43940.958328645836</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>43940.999995312501</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B146">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="C146">
+        <v>4.43</v>
+      </c>
+      <c r="D146">
+        <v>4.43</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>43941.041661979165</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B147">
+        <v>6.49</v>
+      </c>
+      <c r="C147">
+        <v>4.38</v>
+      </c>
+      <c r="D147">
+        <v>4.38</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>43941.083328645836</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B148">
+        <v>4.67</v>
+      </c>
+      <c r="C148">
+        <v>3.69</v>
+      </c>
+      <c r="D148">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>43941.124995312501</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B149">
+        <v>3.98</v>
+      </c>
+      <c r="C149">
+        <v>0.66</v>
+      </c>
+      <c r="D149">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>43941.166661979165</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B150">
+        <v>4.17</v>
+      </c>
+      <c r="C150">
+        <v>0.03</v>
+      </c>
+      <c r="D150">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>43941.208328645836</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B151">
+        <v>9.02</v>
+      </c>
+      <c r="C151">
+        <v>4.78</v>
+      </c>
+      <c r="D151">
+        <v>4.7699999999999996</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>43941.249995312501</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B152">
+        <v>18.940000000000001</v>
+      </c>
+      <c r="C152">
+        <v>18</v>
+      </c>
+      <c r="D152">
+        <v>9.16</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>43941.291661979165</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B153">
+        <v>22.37</v>
+      </c>
+      <c r="C153">
+        <v>22.82</v>
+      </c>
+      <c r="D153">
+        <v>12.77</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>43941.333328645836</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B154">
+        <v>21.94</v>
+      </c>
+      <c r="C154">
+        <v>22.93</v>
+      </c>
+      <c r="D154">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>43941.374995312501</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B155">
+        <v>14.94</v>
+      </c>
+      <c r="C155">
+        <v>16.07</v>
+      </c>
+      <c r="D155">
+        <v>13.97</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>43941.416661979165</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B156">
+        <v>13.52</v>
+      </c>
+      <c r="C156">
+        <v>11.72</v>
+      </c>
+      <c r="D156">
+        <v>12.02</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>43941.458328645836</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B157">
+        <v>13.5</v>
+      </c>
+      <c r="C157">
+        <v>5.46</v>
+      </c>
+      <c r="D157">
+        <v>6.91</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>43941.499995312501</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B158">
+        <v>9.08</v>
+      </c>
+      <c r="C158">
+        <v>-4.9800000000000004</v>
+      </c>
+      <c r="D158">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>43941.541661979165</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B159">
+        <v>6.24</v>
+      </c>
+      <c r="C159">
+        <v>-29.7</v>
+      </c>
+      <c r="D159">
+        <v>-0.09</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>43941.583328645836</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B160">
+        <v>0.79</v>
+      </c>
+      <c r="C160">
+        <v>-44.25</v>
+      </c>
+      <c r="D160">
+        <v>-22.96</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>43941.624995312501</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B161">
+        <v>0.02</v>
+      </c>
+      <c r="C161">
+        <v>-39.49</v>
+      </c>
+      <c r="D161">
+        <v>-23.12</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>43941.666661979165</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B162">
+        <v>1.01</v>
+      </c>
+      <c r="C162">
+        <v>-23.71</v>
+      </c>
+      <c r="D162">
+        <v>-14.63</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>43941.708328645836</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B163">
+        <v>12.84</v>
+      </c>
+      <c r="C163">
+        <v>4.01</v>
+      </c>
+      <c r="D163">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>43941.749995312501</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B164">
+        <v>15.13</v>
+      </c>
+      <c r="C164">
+        <v>16.38</v>
+      </c>
+      <c r="D164">
+        <v>14.23</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>43941.791661979165</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B165">
+        <v>20.41</v>
+      </c>
+      <c r="C165">
+        <v>17.809999999999999</v>
+      </c>
+      <c r="D165">
+        <v>15.02</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>43941.833328645836</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B166">
+        <v>21.6</v>
+      </c>
+      <c r="C166">
+        <v>18.38</v>
+      </c>
+      <c r="D166">
+        <v>15.81</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>43941.874995312501</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B167">
+        <v>18.670000000000002</v>
+      </c>
+      <c r="C167">
+        <v>14.05</v>
+      </c>
+      <c r="D167">
+        <v>14.05</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>43941.916661979165</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B168">
+        <v>15</v>
+      </c>
+      <c r="C168">
+        <v>10.28</v>
+      </c>
+      <c r="D168">
+        <v>13.39</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>43941.958328645836</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B169">
+        <v>13.19</v>
+      </c>
+      <c r="C169">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="D169">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>43941.999995312501</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B170">
+        <v>4.72</v>
+      </c>
+      <c r="C170">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D170">
+        <v>6.31</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>43942.041661979165</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B171">
+        <v>4.29</v>
+      </c>
+      <c r="C171">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="D171">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>43942.083328645836</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B172">
+        <v>1.28</v>
+      </c>
+      <c r="C172">
+        <v>3.69</v>
+      </c>
+      <c r="D172">
+        <v>3.73</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>43942.124995312501</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B173">
+        <v>-1.89</v>
+      </c>
+      <c r="C173">
+        <v>-0.59</v>
+      </c>
+      <c r="D173">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>43942.166661979165</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B174">
+        <v>-0.61</v>
+      </c>
+      <c r="C174">
+        <v>3.72</v>
+      </c>
+      <c r="D174">
+        <v>3.72</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>43942.208328645836</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B175">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="C175">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="D175">
+        <v>4.7300000000000004</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>43942.249995312501</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B176">
+        <v>13.68</v>
+      </c>
+      <c r="C176">
+        <v>10</v>
+      </c>
+      <c r="D176">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>43942.291661979165</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B177">
+        <v>17.28</v>
+      </c>
+      <c r="C177">
+        <v>16.13</v>
+      </c>
+      <c r="D177">
+        <v>11.43</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>43942.333328645836</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B178">
+        <v>17.03</v>
+      </c>
+      <c r="C178">
+        <v>16.52</v>
+      </c>
+      <c r="D178">
+        <v>11.17</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>43942.374995312501</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B179">
+        <v>14.68</v>
+      </c>
+      <c r="C179">
+        <v>7.92</v>
+      </c>
+      <c r="D179">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>43942.416661979165</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B180">
+        <v>13.24</v>
+      </c>
+      <c r="C180">
+        <v>-19.21</v>
+      </c>
+      <c r="D180">
+        <v>-8.65</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>43942.458328645836</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B181">
+        <v>14.69</v>
+      </c>
+      <c r="C181">
+        <v>-69.05</v>
+      </c>
+      <c r="D181">
+        <v>-3.33</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>43942.499995312501</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B182">
+        <v>12.94</v>
+      </c>
+      <c r="C182">
+        <v>-79.739999999999995</v>
+      </c>
+      <c r="D182">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>43942.541661979165</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B183">
+        <v>13.5</v>
+      </c>
+      <c r="C183">
+        <v>-80.09</v>
+      </c>
+      <c r="D183">
+        <v>-0.92</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>43942.583328645836</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B184">
+        <v>13.92</v>
+      </c>
+      <c r="C184">
+        <v>-83.94</v>
+      </c>
+      <c r="D184">
+        <v>-3.99</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>43942.624995312501</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B185">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="C185">
+        <v>-80.02</v>
+      </c>
+      <c r="D185">
+        <v>-8.44</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>43942.666661979165</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B186">
+        <v>9.9</v>
+      </c>
+      <c r="C186">
+        <v>-78.09</v>
+      </c>
+      <c r="D186">
+        <v>-0.09</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>43942.708328645836</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B187">
+        <v>11.5</v>
+      </c>
+      <c r="C187">
+        <v>-23.12</v>
+      </c>
+      <c r="D187">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>43942.749995312501</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B188">
+        <v>13.86</v>
+      </c>
+      <c r="C188">
+        <v>5.53</v>
+      </c>
+      <c r="D188">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>43942.791661979165</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B189">
+        <v>15.2</v>
+      </c>
+      <c r="C189">
+        <v>10.99</v>
+      </c>
+      <c r="D189">
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>43942.833328645836</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B190">
+        <v>16.46</v>
+      </c>
+      <c r="C190">
+        <v>10.99</v>
+      </c>
+      <c r="D190">
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>43942.874995312501</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B191">
+        <v>13.01</v>
+      </c>
+      <c r="C191">
+        <v>11.17</v>
+      </c>
+      <c r="D191">
+        <v>11.17</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>43942.916661979165</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B192">
+        <v>13.69</v>
+      </c>
+      <c r="C192">
+        <v>7.6</v>
+      </c>
+      <c r="D192">
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>43942.958328645836</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B193">
+        <v>9.07</v>
+      </c>
+      <c r="C193">
+        <v>8.31</v>
+      </c>
+      <c r="D193">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>43942.999995312501</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>43943.041661979165</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>43943.083328645836</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>43943.124995312501</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>43943.166661979165</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>43943.208328645836</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>43943.249995312501</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>43943.291661979165</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>43943.333328645836</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>43943.374995312501</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>43943.416661979165</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>43943.458328645836</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>43943.499995312501</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>43943.541661979165</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>43943.583328645836</v>
       </c>

</xml_diff>

<commit_message>
new trans_matrix function implemented and tested
</commit_message>
<xml_diff>
--- a/Spot_Outcomes.xlsx
+++ b/Spot_Outcomes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jens/Documents/Python/dynprog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1248E23-E9DA-8549-9864-91F7E513D9D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609AB784-A95C-8D47-898C-989716376E2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="460" windowWidth="21320" windowHeight="17100" xr2:uid="{97F7539C-452B-A548-92BB-3CE594F78CD0}"/>
   </bookViews>
@@ -686,6 +686,150 @@
                 <c:pt idx="191">
                   <c:v>9.07</c:v>
                 </c:pt>
+                <c:pt idx="192">
+                  <c:v>8.08</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>6.85</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>6.42</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>5.87</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>7.33</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>8.27</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>16.690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>20.67</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>15.07</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>9.09</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>6.74</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>6.68</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>4.67</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>1.62</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>5.82</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>11.16</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>19.47</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>22.37</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>23.19</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>20.67</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>19.57</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>17.670000000000002</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>20.09</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>18.34</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>18.3</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>18.57</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>18.48</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>19.84</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>24.59</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>21.9</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>19.59</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>18.82</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>19.13</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>17.59</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>16.79</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>15.01</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>15.02</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>15.54</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>19.09</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>20.99</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>20.04</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>22.26</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>24.71</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>24.32</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>21.38</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1232,6 +1376,150 @@
                 <c:pt idx="191">
                   <c:v>8.31</c:v>
                 </c:pt>
+                <c:pt idx="192">
+                  <c:v>4.3899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>4.12</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>4.1399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>4.57</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>14.92</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>23.39</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>19.809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>10.57</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>6.77</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>-0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>-24.97</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>-29.98</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>-5.76</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>4.07</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>8.59</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>18.05</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>24.57</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>25.54</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>22.19</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>20.010000000000002</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>20.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>19.68</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>18.38</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>20.07</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>20.6</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>22.34</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>33.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>42.03</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>38.479999999999997</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>23.72</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>18.18</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>17.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>16.95</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>16.63</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>14.95</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>14.97</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>18.11</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>25.07</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>34.51</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>58.95</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>69.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>38.619999999999997</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>34.43</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>28.6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1777,6 +2065,150 @@
                 </c:pt>
                 <c:pt idx="191">
                   <c:v>9.99</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>4.6399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>4.12</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>4.1399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>4.57</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>8.49</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>11.64</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>10.57</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>6.77</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>5.62</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>-5.72</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>-0.78</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>4.07</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>8.59</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>12.14</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>18.850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>20.03</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>22.19</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>20.010000000000002</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>20.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>18.61</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>16.11</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>13.49</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>12.69</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>14.01</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>14.55</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>16.16</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>19.02</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>20.010000000000002</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>18.18</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>17.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>16.95</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>16.63</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>14.95</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>14.97</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>14.79</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>16.73</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>18.850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>21.33</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>22.4</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>23.94</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>22.31</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>21.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2885,8 +3317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2513C063-BB01-5E4E-BC20-809D3836ED8C}">
   <dimension ref="A1:D271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="W38" sqref="W38"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="B243" sqref="B243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5384,313 +5816,745 @@
       <c r="A194" s="1">
         <v>43942.999995312501</v>
       </c>
+      <c r="B194">
+        <v>8.08</v>
+      </c>
+      <c r="C194">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="D194">
+        <v>4.6399999999999997</v>
+      </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>43943.041661979165</v>
       </c>
+      <c r="B195">
+        <v>6.85</v>
+      </c>
+      <c r="C195">
+        <v>4.12</v>
+      </c>
+      <c r="D195">
+        <v>4.12</v>
+      </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>43943.083328645836</v>
       </c>
+      <c r="B196">
+        <v>6.42</v>
+      </c>
+      <c r="C196">
+        <v>3.5</v>
+      </c>
+      <c r="D196">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>43943.124995312501</v>
       </c>
+      <c r="B197">
+        <v>5.87</v>
+      </c>
+      <c r="C197">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="D197">
+        <v>4.1399999999999997</v>
+      </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>43943.166661979165</v>
       </c>
+      <c r="B198">
+        <v>7.33</v>
+      </c>
+      <c r="C198">
+        <v>4.57</v>
+      </c>
+      <c r="D198">
+        <v>4.57</v>
+      </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>43943.208328645836</v>
       </c>
+      <c r="B199">
+        <v>8.27</v>
+      </c>
+      <c r="C199">
+        <v>6</v>
+      </c>
+      <c r="D199">
+        <v>6</v>
+      </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>43943.249995312501</v>
       </c>
+      <c r="B200">
+        <v>16.690000000000001</v>
+      </c>
+      <c r="C200">
+        <v>14.92</v>
+      </c>
+      <c r="D200">
+        <v>8</v>
+      </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>43943.291661979165</v>
       </c>
+      <c r="B201">
+        <v>20.67</v>
+      </c>
+      <c r="C201">
+        <v>23.39</v>
+      </c>
+      <c r="D201">
+        <v>8.49</v>
+      </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>43943.333328645836</v>
       </c>
+      <c r="B202">
+        <v>21</v>
+      </c>
+      <c r="C202">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="D202">
+        <v>11.64</v>
+      </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>43943.374995312501</v>
       </c>
+      <c r="B203">
+        <v>15.07</v>
+      </c>
+      <c r="C203">
+        <v>10.57</v>
+      </c>
+      <c r="D203">
+        <v>10.57</v>
+      </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>43943.416661979165</v>
       </c>
+      <c r="B204">
+        <v>9.09</v>
+      </c>
+      <c r="C204">
+        <v>6.77</v>
+      </c>
+      <c r="D204">
+        <v>6.77</v>
+      </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>43943.458328645836</v>
       </c>
+      <c r="B205">
+        <v>6.74</v>
+      </c>
+      <c r="C205">
+        <v>6.1</v>
+      </c>
+      <c r="D205">
+        <v>6.1</v>
+      </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>43943.499995312501</v>
       </c>
+      <c r="B206">
+        <v>6.68</v>
+      </c>
+      <c r="C206">
+        <v>-0.56000000000000005</v>
+      </c>
+      <c r="D206">
+        <v>5.62</v>
+      </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>43943.541661979165</v>
       </c>
+      <c r="B207">
+        <v>4.67</v>
+      </c>
+      <c r="C207">
+        <v>-24.97</v>
+      </c>
+      <c r="D207">
+        <v>3.14</v>
+      </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>43943.583328645836</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B208">
+        <v>0.94</v>
+      </c>
+      <c r="C208">
+        <v>-29.98</v>
+      </c>
+      <c r="D208">
+        <v>-5.72</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>43943.624995312501</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B209">
+        <v>1.62</v>
+      </c>
+      <c r="C209">
+        <v>-5.76</v>
+      </c>
+      <c r="D209">
+        <v>-0.78</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>43943.666661979165</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B210">
+        <v>5.82</v>
+      </c>
+      <c r="C210">
+        <v>4.07</v>
+      </c>
+      <c r="D210">
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>43943.708328645836</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B211">
+        <v>11.16</v>
+      </c>
+      <c r="C211">
+        <v>8.59</v>
+      </c>
+      <c r="D211">
+        <v>8.59</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>43943.749995312501</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B212">
+        <v>19.47</v>
+      </c>
+      <c r="C212">
+        <v>18.05</v>
+      </c>
+      <c r="D212">
+        <v>12.14</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>43943.791661979165</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B213">
+        <v>22.37</v>
+      </c>
+      <c r="C213">
+        <v>24.57</v>
+      </c>
+      <c r="D213">
+        <v>18.850000000000001</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>43943.833328645836</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B214">
+        <v>23.19</v>
+      </c>
+      <c r="C214">
+        <v>25.54</v>
+      </c>
+      <c r="D214">
+        <v>20.03</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>43943.874995312501</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B215">
+        <v>20.67</v>
+      </c>
+      <c r="C215">
+        <v>22.19</v>
+      </c>
+      <c r="D215">
+        <v>22.19</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>43943.916661979165</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B216">
+        <v>19.57</v>
+      </c>
+      <c r="C216">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="D216">
+        <v>20.010000000000002</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>43943.958328645836</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B217">
+        <v>17.670000000000002</v>
+      </c>
+      <c r="C217">
+        <v>19</v>
+      </c>
+      <c r="D217">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>43943.999995312501</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B218">
+        <v>20.09</v>
+      </c>
+      <c r="C218">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="D218">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>43944.041661979165</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B219">
+        <v>18.34</v>
+      </c>
+      <c r="C219">
+        <v>19.68</v>
+      </c>
+      <c r="D219">
+        <v>18.61</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>43944.083328645836</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B220">
+        <v>18.3</v>
+      </c>
+      <c r="C220">
+        <v>18.38</v>
+      </c>
+      <c r="D220">
+        <v>16.11</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>43944.124995312501</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B221">
+        <v>18.57</v>
+      </c>
+      <c r="C221">
+        <v>20.07</v>
+      </c>
+      <c r="D221">
+        <v>13.49</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>43944.166661979165</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B222">
+        <v>18.48</v>
+      </c>
+      <c r="C222">
+        <v>20.6</v>
+      </c>
+      <c r="D222">
+        <v>12.69</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>43944.208328645836</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B223">
+        <v>19.84</v>
+      </c>
+      <c r="C223">
+        <v>22.34</v>
+      </c>
+      <c r="D223">
+        <v>14.01</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>43944.249995312501</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B224">
+        <v>24.59</v>
+      </c>
+      <c r="C224">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="D224">
+        <v>14.55</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>43944.291661979165</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B225">
+        <v>21.9</v>
+      </c>
+      <c r="C225">
+        <v>42.03</v>
+      </c>
+      <c r="D225">
+        <v>16.16</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>43944.333328645836</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B226">
+        <v>22</v>
+      </c>
+      <c r="C226">
+        <v>38.479999999999997</v>
+      </c>
+      <c r="D226">
+        <v>19.02</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>43944.374995312501</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B227">
+        <v>19.59</v>
+      </c>
+      <c r="C227">
+        <v>23.72</v>
+      </c>
+      <c r="D227">
+        <v>20.010000000000002</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>43944.416661979165</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B228">
+        <v>18.82</v>
+      </c>
+      <c r="C228">
+        <v>18.18</v>
+      </c>
+      <c r="D228">
+        <v>18.18</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>43944.458328645836</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B229">
+        <v>19.13</v>
+      </c>
+      <c r="C229">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D229">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>43944.499995312501</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B230">
+        <v>17.59</v>
+      </c>
+      <c r="C230">
+        <v>16.95</v>
+      </c>
+      <c r="D230">
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>43944.541661979165</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B231">
+        <v>16.79</v>
+      </c>
+      <c r="C231">
+        <v>16.63</v>
+      </c>
+      <c r="D231">
+        <v>16.63</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>43944.583328645836</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B232">
+        <v>15.01</v>
+      </c>
+      <c r="C232">
+        <v>14.95</v>
+      </c>
+      <c r="D232">
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>43944.624995312501</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B233">
+        <v>15.02</v>
+      </c>
+      <c r="C233">
+        <v>14.97</v>
+      </c>
+      <c r="D233">
+        <v>14.97</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>43944.666661979165</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B234">
+        <v>15.54</v>
+      </c>
+      <c r="C234">
+        <v>18.11</v>
+      </c>
+      <c r="D234">
+        <v>14.79</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>43944.708328645836</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B235">
+        <v>19.09</v>
+      </c>
+      <c r="C235">
+        <v>25.07</v>
+      </c>
+      <c r="D235">
+        <v>16.73</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>43944.749995312501</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B236">
+        <v>20.99</v>
+      </c>
+      <c r="C236">
+        <v>34.51</v>
+      </c>
+      <c r="D236">
+        <v>18.850000000000001</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>43944.791661979165</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B237">
+        <v>20.04</v>
+      </c>
+      <c r="C237">
+        <v>58.95</v>
+      </c>
+      <c r="D237">
+        <v>21.33</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>43944.833328645836</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B238">
+        <v>22.26</v>
+      </c>
+      <c r="C238">
+        <v>69.680000000000007</v>
+      </c>
+      <c r="D238">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>43944.874995312501</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B239">
+        <v>24.71</v>
+      </c>
+      <c r="C239">
+        <v>38.619999999999997</v>
+      </c>
+      <c r="D239">
+        <v>23.94</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>43944.916661979165</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B240">
+        <v>24.32</v>
+      </c>
+      <c r="C240">
+        <v>34.43</v>
+      </c>
+      <c r="D240">
+        <v>22.31</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>43944.958328645836</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B241">
+        <v>21.38</v>
+      </c>
+      <c r="C241">
+        <v>28.6</v>
+      </c>
+      <c r="D241">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>43944.999995312501</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>43945.041661979165</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>43945.083328645836</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>43945.124995312501</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>43945.166661979165</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>43945.208328645836</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>43945.249995312501</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>43945.291661979165</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>43945.333328645836</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>43945.374995312501</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>43945.416661979165</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>43945.458328645836</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>43945.499995312501</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>43945.541661979165</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>43945.583328645836</v>
       </c>

</xml_diff>